<commit_message>
Drop duplicate rows in geological 'FlowablePrimaryContexts'
</commit_message>
<xml_diff>
--- a/fedelemflowlist/input/Geological.xlsx
+++ b/fedelemflowlist/input/Geological.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wesle\Federal-LCA-Commons-Elementary-Flow-List\fedelemflowlist\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wingwers\Federal-LCA-Commons-Elementary-Flow-List\fedelemflowlist\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68055E1-2D6D-436B-B83D-999F8A16C9D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3C1B3C-E5AD-4625-8E4E-66D9D035FFA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -43,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4303" uniqueCount="1403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4270" uniqueCount="1403">
   <si>
     <t>CAS No</t>
   </si>
@@ -15670,9 +15669,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C487"/>
+  <dimension ref="A1:C476"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="A140" sqref="A140"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -15760,7 +15761,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1374</v>
+        <v>103</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -15771,7 +15772,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1372</v>
+        <v>1374</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -15782,7 +15783,7 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1369</v>
+        <v>1372</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -15793,7 +15794,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1366</v>
+        <v>1369</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -15804,18 +15805,18 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>1366</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
         <v>45</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>1361</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
@@ -15826,7 +15827,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1359</v>
+        <v>1361</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
@@ -15837,7 +15838,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1356</v>
+        <v>1359</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
@@ -15848,7 +15849,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1354</v>
+        <v>1356</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
@@ -15859,7 +15860,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1351</v>
+        <v>102</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -15870,7 +15871,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1348</v>
+        <v>1354</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
@@ -15881,7 +15882,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>1346</v>
+        <v>1351</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
@@ -15892,7 +15893,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1344</v>
+        <v>1348</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
@@ -15903,7 +15904,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1341</v>
+        <v>1346</v>
       </c>
       <c r="B21" t="s">
         <v>6</v>
@@ -15914,7 +15915,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1338</v>
+        <v>1344</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
@@ -15925,7 +15926,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1335</v>
+        <v>1341</v>
       </c>
       <c r="B23" t="s">
         <v>6</v>
@@ -15936,7 +15937,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1332</v>
+        <v>1338</v>
       </c>
       <c r="B24" t="s">
         <v>6</v>
@@ -15947,7 +15948,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1330</v>
+        <v>1335</v>
       </c>
       <c r="B25" t="s">
         <v>6</v>
@@ -15958,7 +15959,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1328</v>
+        <v>1332</v>
       </c>
       <c r="B26" t="s">
         <v>6</v>
@@ -15969,18 +15970,18 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1325</v>
+        <v>1330</v>
       </c>
       <c r="B27" t="s">
         <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>1392</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1321</v>
+        <v>1328</v>
       </c>
       <c r="B28" t="s">
         <v>6</v>
@@ -15991,18 +15992,18 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1318</v>
+        <v>1325</v>
       </c>
       <c r="B29" t="s">
         <v>6</v>
       </c>
       <c r="C29" t="s">
-        <v>8</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>1315</v>
+        <v>1321</v>
       </c>
       <c r="B30" t="s">
         <v>6</v>
@@ -16013,7 +16014,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>1312</v>
+        <v>1318</v>
       </c>
       <c r="B31" t="s">
         <v>6</v>
@@ -16024,7 +16025,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1309</v>
+        <v>1315</v>
       </c>
       <c r="B32" t="s">
         <v>6</v>
@@ -16035,7 +16036,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1306</v>
+        <v>1312</v>
       </c>
       <c r="B33" t="s">
         <v>6</v>
@@ -16045,8 +16046,8 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>1303</v>
+      <c r="A34" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="B34" t="s">
         <v>6</v>
@@ -16057,7 +16058,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>1299</v>
+        <v>1309</v>
       </c>
       <c r="B35" t="s">
         <v>6</v>
@@ -16068,7 +16069,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>48</v>
+        <v>1306</v>
       </c>
       <c r="B36" t="s">
         <v>6</v>
@@ -16079,7 +16080,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>1295</v>
+        <v>1303</v>
       </c>
       <c r="B37" t="s">
         <v>6</v>
@@ -16090,7 +16091,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>1292</v>
+        <v>1299</v>
       </c>
       <c r="B38" t="s">
         <v>6</v>
@@ -16101,7 +16102,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>1289</v>
+        <v>48</v>
       </c>
       <c r="B39" t="s">
         <v>6</v>
@@ -16112,7 +16113,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>1286</v>
+        <v>1292</v>
       </c>
       <c r="B40" t="s">
         <v>6</v>
@@ -16123,7 +16124,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>1283</v>
+        <v>1295</v>
       </c>
       <c r="B41" t="s">
         <v>6</v>
@@ -16134,7 +16135,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>1279</v>
+        <v>1289</v>
       </c>
       <c r="B42" t="s">
         <v>6</v>
@@ -16145,7 +16146,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>1277</v>
+        <v>1271</v>
       </c>
       <c r="B43" t="s">
         <v>6</v>
@@ -16156,7 +16157,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>1275</v>
+        <v>1283</v>
       </c>
       <c r="B44" t="s">
         <v>6</v>
@@ -16167,7 +16168,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>1271</v>
+        <v>1279</v>
       </c>
       <c r="B45" t="s">
         <v>6</v>
@@ -16178,7 +16179,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>1269</v>
+        <v>1277</v>
       </c>
       <c r="B46" t="s">
         <v>6</v>
@@ -16189,7 +16190,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>1267</v>
+        <v>1275</v>
       </c>
       <c r="B47" t="s">
         <v>6</v>
@@ -16200,7 +16201,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>1264</v>
+        <v>1286</v>
       </c>
       <c r="B48" t="s">
         <v>6</v>
@@ -16211,7 +16212,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>1261</v>
+        <v>1269</v>
       </c>
       <c r="B49" t="s">
         <v>6</v>
@@ -16222,7 +16223,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>1258</v>
+        <v>1267</v>
       </c>
       <c r="B50" t="s">
         <v>6</v>
@@ -16233,7 +16234,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>1255</v>
+        <v>1264</v>
       </c>
       <c r="B51" t="s">
         <v>6</v>
@@ -16244,7 +16245,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>1252</v>
+        <v>1261</v>
       </c>
       <c r="B52" t="s">
         <v>6</v>
@@ -16255,7 +16256,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>1248</v>
+        <v>1258</v>
       </c>
       <c r="B53" t="s">
         <v>6</v>
@@ -16266,7 +16267,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>1245</v>
+        <v>1255</v>
       </c>
       <c r="B54" t="s">
         <v>6</v>
@@ -16277,7 +16278,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>1242</v>
+        <v>1252</v>
       </c>
       <c r="B55" t="s">
         <v>6</v>
@@ -16288,7 +16289,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>1239</v>
+        <v>1248</v>
       </c>
       <c r="B56" t="s">
         <v>6</v>
@@ -16299,7 +16300,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>1237</v>
+        <v>1245</v>
       </c>
       <c r="B57" t="s">
         <v>6</v>
@@ -16310,7 +16311,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>1233</v>
+        <v>1242</v>
       </c>
       <c r="B58" t="s">
         <v>6</v>
@@ -16321,7 +16322,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>1229</v>
+        <v>1239</v>
       </c>
       <c r="B59" t="s">
         <v>6</v>
@@ -16332,7 +16333,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>47</v>
+        <v>1237</v>
       </c>
       <c r="B60" t="s">
         <v>6</v>
@@ -16343,7 +16344,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>1224</v>
+        <v>1233</v>
       </c>
       <c r="B61" t="s">
         <v>6</v>
@@ -16354,7 +16355,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>1221</v>
+        <v>1229</v>
       </c>
       <c r="B62" t="s">
         <v>6</v>
@@ -16364,8 +16365,8 @@
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>41</v>
+      <c r="A63" s="13" t="s">
+        <v>47</v>
       </c>
       <c r="B63" t="s">
         <v>6</v>
@@ -16376,7 +16377,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>41</v>
+        <v>1224</v>
       </c>
       <c r="B64" t="s">
         <v>6</v>
@@ -16387,7 +16388,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>1214</v>
+        <v>1221</v>
       </c>
       <c r="B65" t="s">
         <v>6</v>
@@ -16398,7 +16399,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>1211</v>
+        <v>41</v>
       </c>
       <c r="B66" t="s">
         <v>6</v>
@@ -16408,19 +16409,19 @@
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>1208</v>
+      <c r="A67" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="B67" t="s">
         <v>6</v>
       </c>
       <c r="C67" t="s">
-        <v>8</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>1206</v>
+        <v>1214</v>
       </c>
       <c r="B68" t="s">
         <v>6</v>
@@ -16431,7 +16432,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>1203</v>
+        <v>1211</v>
       </c>
       <c r="B69" t="s">
         <v>6</v>
@@ -16442,7 +16443,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>1202</v>
+        <v>1208</v>
       </c>
       <c r="B70" t="s">
         <v>6</v>
@@ -16453,7 +16454,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>1199</v>
+        <v>1206</v>
       </c>
       <c r="B71" t="s">
         <v>6</v>
@@ -16464,7 +16465,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>1196</v>
+        <v>1203</v>
       </c>
       <c r="B72" t="s">
         <v>6</v>
@@ -16475,7 +16476,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>85</v>
+        <v>46</v>
       </c>
       <c r="B73" t="s">
         <v>6</v>
@@ -16486,7 +16487,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>81</v>
+        <v>1202</v>
       </c>
       <c r="B74" t="s">
         <v>6</v>
@@ -16497,7 +16498,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>77</v>
+        <v>1199</v>
       </c>
       <c r="B75" t="s">
         <v>6</v>
@@ -16508,7 +16509,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>1190</v>
+        <v>1196</v>
       </c>
       <c r="B76" t="s">
         <v>6</v>
@@ -16519,18 +16520,18 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>1187</v>
+        <v>85</v>
       </c>
       <c r="B77" t="s">
         <v>6</v>
       </c>
       <c r="C77" t="s">
-        <v>1392</v>
+        <v>8</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>1184</v>
+        <v>81</v>
       </c>
       <c r="B78" t="s">
         <v>6</v>
@@ -16541,7 +16542,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>1180</v>
+        <v>83</v>
       </c>
       <c r="B79" t="s">
         <v>6</v>
@@ -16552,7 +16553,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>1177</v>
+        <v>77</v>
       </c>
       <c r="B80" t="s">
         <v>6</v>
@@ -16563,7 +16564,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>1174</v>
+        <v>79</v>
       </c>
       <c r="B81" t="s">
         <v>6</v>
@@ -16574,7 +16575,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>1171</v>
+        <v>1190</v>
       </c>
       <c r="B82" t="s">
         <v>6</v>
@@ -16585,7 +16586,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>1169</v>
+        <v>75</v>
       </c>
       <c r="B83" t="s">
         <v>6</v>
@@ -16596,18 +16597,18 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>46</v>
+        <v>1187</v>
       </c>
       <c r="B84" t="s">
         <v>6</v>
       </c>
       <c r="C84" t="s">
-        <v>8</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>1164</v>
+        <v>1184</v>
       </c>
       <c r="B85" t="s">
         <v>6</v>
@@ -16618,7 +16619,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>1161</v>
+        <v>1180</v>
       </c>
       <c r="B86" t="s">
         <v>6</v>
@@ -16629,7 +16630,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>1158</v>
+        <v>1177</v>
       </c>
       <c r="B87" t="s">
         <v>6</v>
@@ -16640,7 +16641,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>42</v>
+        <v>1174</v>
       </c>
       <c r="B88" t="s">
         <v>6</v>
@@ -16651,7 +16652,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>1154</v>
+        <v>1171</v>
       </c>
       <c r="B89" t="s">
         <v>6</v>
@@ -16662,7 +16663,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>1151</v>
+        <v>1169</v>
       </c>
       <c r="B90" t="s">
         <v>6</v>
@@ -16673,7 +16674,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>1148</v>
+        <v>1164</v>
       </c>
       <c r="B91" t="s">
         <v>6</v>
@@ -16684,7 +16685,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>1145</v>
+        <v>1161</v>
       </c>
       <c r="B92" t="s">
         <v>6</v>
@@ -16695,7 +16696,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>1141</v>
+        <v>1158</v>
       </c>
       <c r="B93" t="s">
         <v>6</v>
@@ -16706,7 +16707,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>1137</v>
+        <v>42</v>
       </c>
       <c r="B94" t="s">
         <v>6</v>
@@ -16717,7 +16718,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>1134</v>
+        <v>1154</v>
       </c>
       <c r="B95" t="s">
         <v>6</v>
@@ -16728,7 +16729,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>1131</v>
+        <v>1151</v>
       </c>
       <c r="B96" t="s">
         <v>6</v>
@@ -16739,7 +16740,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>1127</v>
+        <v>1148</v>
       </c>
       <c r="B97" t="s">
         <v>6</v>
@@ -16750,7 +16751,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>1124</v>
+        <v>1145</v>
       </c>
       <c r="B98" t="s">
         <v>6</v>
@@ -16761,7 +16762,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>1121</v>
+        <v>1141</v>
       </c>
       <c r="B99" t="s">
         <v>6</v>
@@ -16772,7 +16773,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>1118</v>
+        <v>1137</v>
       </c>
       <c r="B100" t="s">
         <v>6</v>
@@ -16783,7 +16784,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>1116</v>
+        <v>1134</v>
       </c>
       <c r="B101" t="s">
         <v>6</v>
@@ -16794,7 +16795,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>1112</v>
+        <v>1131</v>
       </c>
       <c r="B102" t="s">
         <v>6</v>
@@ -16805,7 +16806,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>1109</v>
+        <v>1127</v>
       </c>
       <c r="B103" t="s">
         <v>6</v>
@@ -16816,7 +16817,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>1106</v>
+        <v>1124</v>
       </c>
       <c r="B104" t="s">
         <v>6</v>
@@ -16827,7 +16828,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>1104</v>
+        <v>1121</v>
       </c>
       <c r="B105" t="s">
         <v>6</v>
@@ -16838,7 +16839,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>1101</v>
+        <v>1118</v>
       </c>
       <c r="B106" t="s">
         <v>6</v>
@@ -16849,7 +16850,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>1098</v>
+        <v>52</v>
       </c>
       <c r="B107" t="s">
         <v>6</v>
@@ -16860,7 +16861,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>1095</v>
+        <v>61</v>
       </c>
       <c r="B108" t="s">
         <v>6</v>
@@ -16871,7 +16872,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>1092</v>
+        <v>62</v>
       </c>
       <c r="B109" t="s">
         <v>6</v>
@@ -16882,7 +16883,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B110" t="s">
         <v>6</v>
@@ -16892,8 +16893,8 @@
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>1087</v>
+      <c r="A111" s="13" t="s">
+        <v>1394</v>
       </c>
       <c r="B111" t="s">
         <v>6</v>
@@ -16904,7 +16905,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>1084</v>
+        <v>60</v>
       </c>
       <c r="B112" t="s">
         <v>6</v>
@@ -16915,7 +16916,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>1081</v>
+        <v>1116</v>
       </c>
       <c r="B113" t="s">
         <v>6</v>
@@ -16926,7 +16927,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>1078</v>
+        <v>1112</v>
       </c>
       <c r="B114" t="s">
         <v>6</v>
@@ -16937,7 +16938,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>1075</v>
+        <v>1109</v>
       </c>
       <c r="B115" t="s">
         <v>6</v>
@@ -16948,7 +16949,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>1072</v>
+        <v>1104</v>
       </c>
       <c r="B116" t="s">
         <v>6</v>
@@ -16959,7 +16960,7 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>1069</v>
+        <v>1101</v>
       </c>
       <c r="B117" t="s">
         <v>6</v>
@@ -16970,7 +16971,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>1066</v>
+        <v>1106</v>
       </c>
       <c r="B118" t="s">
         <v>6</v>
@@ -16981,7 +16982,7 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>1064</v>
+        <v>1098</v>
       </c>
       <c r="B119" t="s">
         <v>6</v>
@@ -16991,8 +16992,8 @@
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>1061</v>
+      <c r="A120" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="B120" t="s">
         <v>6</v>
@@ -17003,7 +17004,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>1059</v>
+        <v>1095</v>
       </c>
       <c r="B121" t="s">
         <v>6</v>
@@ -17014,7 +17015,7 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>1056</v>
+        <v>1092</v>
       </c>
       <c r="B122" t="s">
         <v>6</v>
@@ -17025,7 +17026,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>1054</v>
+        <v>1087</v>
       </c>
       <c r="B123" t="s">
         <v>6</v>
@@ -17036,7 +17037,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>1050</v>
+        <v>1084</v>
       </c>
       <c r="B124" t="s">
         <v>6</v>
@@ -17047,7 +17048,7 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>1047</v>
+        <v>1081</v>
       </c>
       <c r="B125" t="s">
         <v>6</v>
@@ -17058,7 +17059,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>1043</v>
+        <v>1078</v>
       </c>
       <c r="B126" t="s">
         <v>6</v>
@@ -17069,18 +17070,18 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>1040</v>
+        <v>59</v>
       </c>
       <c r="B127" t="s">
         <v>6</v>
       </c>
       <c r="C127" t="s">
-        <v>8</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>1037</v>
+        <v>1075</v>
       </c>
       <c r="B128" t="s">
         <v>6</v>
@@ -17091,7 +17092,7 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>1034</v>
+        <v>1072</v>
       </c>
       <c r="B129" t="s">
         <v>6</v>
@@ -17102,7 +17103,7 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>1031</v>
+        <v>1069</v>
       </c>
       <c r="B130" t="s">
         <v>6</v>
@@ -17113,7 +17114,7 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>1028</v>
+        <v>1066</v>
       </c>
       <c r="B131" t="s">
         <v>6</v>
@@ -17124,7 +17125,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>1025</v>
+        <v>1064</v>
       </c>
       <c r="B132" t="s">
         <v>6</v>
@@ -17135,7 +17136,7 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>1022</v>
+        <v>1061</v>
       </c>
       <c r="B133" t="s">
         <v>6</v>
@@ -17146,7 +17147,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>1019</v>
+        <v>1059</v>
       </c>
       <c r="B134" t="s">
         <v>6</v>
@@ -17157,7 +17158,7 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>1016</v>
+        <v>1056</v>
       </c>
       <c r="B135" t="s">
         <v>6</v>
@@ -17168,7 +17169,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>1013</v>
+        <v>1054</v>
       </c>
       <c r="B136" t="s">
         <v>6</v>
@@ -17179,7 +17180,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>1010</v>
+        <v>1050</v>
       </c>
       <c r="B137" t="s">
         <v>6</v>
@@ -17190,7 +17191,7 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>50</v>
+        <v>1047</v>
       </c>
       <c r="B138" t="s">
         <v>6</v>
@@ -17201,7 +17202,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>1006</v>
+        <v>1043</v>
       </c>
       <c r="B139" t="s">
         <v>6</v>
@@ -17212,7 +17213,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>1003</v>
+        <v>1040</v>
       </c>
       <c r="B140" t="s">
         <v>6</v>
@@ -17223,7 +17224,7 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>1000</v>
+        <v>1037</v>
       </c>
       <c r="B141" t="s">
         <v>6</v>
@@ -17234,7 +17235,7 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>997</v>
+        <v>1034</v>
       </c>
       <c r="B142" t="s">
         <v>6</v>
@@ -17245,7 +17246,7 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>49</v>
+        <v>1031</v>
       </c>
       <c r="B143" t="s">
         <v>6</v>
@@ -17256,7 +17257,7 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>993</v>
+        <v>1028</v>
       </c>
       <c r="B144" t="s">
         <v>6</v>
@@ -17267,7 +17268,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>991</v>
+        <v>1025</v>
       </c>
       <c r="B145" t="s">
         <v>6</v>
@@ -17278,7 +17279,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>987</v>
+        <v>1022</v>
       </c>
       <c r="B146" t="s">
         <v>6</v>
@@ -17289,7 +17290,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>984</v>
+        <v>1019</v>
       </c>
       <c r="B147" t="s">
         <v>6</v>
@@ -17300,7 +17301,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>981</v>
+        <v>1016</v>
       </c>
       <c r="B148" t="s">
         <v>6</v>
@@ -17311,7 +17312,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>978</v>
+        <v>1013</v>
       </c>
       <c r="B149" t="s">
         <v>6</v>
@@ -17322,7 +17323,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>975</v>
+        <v>1010</v>
       </c>
       <c r="B150" t="s">
         <v>6</v>
@@ -17332,8 +17333,8 @@
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>972</v>
+      <c r="A151" s="13" t="s">
+        <v>50</v>
       </c>
       <c r="B151" t="s">
         <v>6</v>
@@ -17344,7 +17345,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>969</v>
+        <v>1006</v>
       </c>
       <c r="B152" t="s">
         <v>6</v>
@@ -17355,7 +17356,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>966</v>
+        <v>1003</v>
       </c>
       <c r="B153" t="s">
         <v>6</v>
@@ -17366,7 +17367,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>964</v>
+        <v>1000</v>
       </c>
       <c r="B154" t="s">
         <v>6</v>
@@ -17377,7 +17378,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>960</v>
+        <v>997</v>
       </c>
       <c r="B155" t="s">
         <v>6</v>
@@ -17387,8 +17388,8 @@
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
-        <v>957</v>
+      <c r="A156" s="13" t="s">
+        <v>49</v>
       </c>
       <c r="B156" t="s">
         <v>6</v>
@@ -17399,7 +17400,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>953</v>
+        <v>993</v>
       </c>
       <c r="B157" t="s">
         <v>6</v>
@@ -17410,7 +17411,7 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>950</v>
+        <v>991</v>
       </c>
       <c r="B158" t="s">
         <v>6</v>
@@ -17421,7 +17422,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>947</v>
+        <v>987</v>
       </c>
       <c r="B159" t="s">
         <v>6</v>
@@ -17432,7 +17433,7 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>944</v>
+        <v>984</v>
       </c>
       <c r="B160" t="s">
         <v>6</v>
@@ -17443,7 +17444,7 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>941</v>
+        <v>981</v>
       </c>
       <c r="B161" t="s">
         <v>6</v>
@@ -17454,7 +17455,7 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>938</v>
+        <v>978</v>
       </c>
       <c r="B162" t="s">
         <v>6</v>
@@ -17465,7 +17466,7 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>935</v>
+        <v>975</v>
       </c>
       <c r="B163" t="s">
         <v>6</v>
@@ -17476,7 +17477,7 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>932</v>
+        <v>972</v>
       </c>
       <c r="B164" t="s">
         <v>6</v>
@@ -17487,7 +17488,7 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>929</v>
+        <v>969</v>
       </c>
       <c r="B165" t="s">
         <v>6</v>
@@ -17498,7 +17499,7 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>927</v>
+        <v>966</v>
       </c>
       <c r="B166" t="s">
         <v>6</v>
@@ -17509,7 +17510,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>923</v>
+        <v>964</v>
       </c>
       <c r="B167" t="s">
         <v>6</v>
@@ -17520,7 +17521,7 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>921</v>
+        <v>960</v>
       </c>
       <c r="B168" t="s">
         <v>6</v>
@@ -17531,7 +17532,7 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>918</v>
+        <v>957</v>
       </c>
       <c r="B169" t="s">
         <v>6</v>
@@ -17542,7 +17543,7 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>916</v>
+        <v>953</v>
       </c>
       <c r="B170" t="s">
         <v>6</v>
@@ -17553,7 +17554,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>913</v>
+        <v>950</v>
       </c>
       <c r="B171" t="s">
         <v>6</v>
@@ -17564,7 +17565,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>910</v>
+        <v>947</v>
       </c>
       <c r="B172" t="s">
         <v>6</v>
@@ -17575,7 +17576,7 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>907</v>
+        <v>944</v>
       </c>
       <c r="B173" t="s">
         <v>6</v>
@@ -17586,7 +17587,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>905</v>
+        <v>941</v>
       </c>
       <c r="B174" t="s">
         <v>6</v>
@@ -17597,7 +17598,7 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>902</v>
+        <v>938</v>
       </c>
       <c r="B175" t="s">
         <v>6</v>
@@ -17608,7 +17609,7 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>899</v>
+        <v>935</v>
       </c>
       <c r="B176" t="s">
         <v>6</v>
@@ -17619,7 +17620,7 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>897</v>
+        <v>932</v>
       </c>
       <c r="B177" t="s">
         <v>6</v>
@@ -17630,7 +17631,7 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>894</v>
+        <v>929</v>
       </c>
       <c r="B178" t="s">
         <v>6</v>
@@ -17641,18 +17642,18 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>890</v>
+        <v>927</v>
       </c>
       <c r="B179" t="s">
         <v>6</v>
       </c>
       <c r="C179" t="s">
-        <v>1392</v>
+        <v>8</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>886</v>
+        <v>923</v>
       </c>
       <c r="B180" t="s">
         <v>6</v>
@@ -17663,7 +17664,7 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>883</v>
+        <v>921</v>
       </c>
       <c r="B181" t="s">
         <v>6</v>
@@ -17674,7 +17675,7 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>880</v>
+        <v>918</v>
       </c>
       <c r="B182" t="s">
         <v>6</v>
@@ -17685,7 +17686,7 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>877</v>
+        <v>916</v>
       </c>
       <c r="B183" t="s">
         <v>6</v>
@@ -17696,7 +17697,7 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>874</v>
+        <v>913</v>
       </c>
       <c r="B184" t="s">
         <v>6</v>
@@ -17706,8 +17707,8 @@
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
-        <v>871</v>
+      <c r="A185" s="13" t="s">
+        <v>40</v>
       </c>
       <c r="B185" t="s">
         <v>6</v>
@@ -17718,7 +17719,7 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>868</v>
+        <v>910</v>
       </c>
       <c r="B186" t="s">
         <v>6</v>
@@ -17729,7 +17730,7 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>865</v>
+        <v>907</v>
       </c>
       <c r="B187" t="s">
         <v>6</v>
@@ -17740,7 +17741,7 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>862</v>
+        <v>905</v>
       </c>
       <c r="B188" t="s">
         <v>6</v>
@@ -17751,7 +17752,7 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>859</v>
+        <v>902</v>
       </c>
       <c r="B189" t="s">
         <v>6</v>
@@ -17762,7 +17763,7 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>856</v>
+        <v>899</v>
       </c>
       <c r="B190" t="s">
         <v>6</v>
@@ -17773,7 +17774,7 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>853</v>
+        <v>897</v>
       </c>
       <c r="B191" t="s">
         <v>6</v>
@@ -17784,7 +17785,7 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>849</v>
+        <v>894</v>
       </c>
       <c r="B192" t="s">
         <v>6</v>
@@ -17795,18 +17796,18 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>845</v>
+        <v>890</v>
       </c>
       <c r="B193" t="s">
         <v>6</v>
       </c>
       <c r="C193" t="s">
-        <v>8</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>842</v>
+        <v>886</v>
       </c>
       <c r="B194" t="s">
         <v>6</v>
@@ -17817,7 +17818,7 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>839</v>
+        <v>883</v>
       </c>
       <c r="B195" t="s">
         <v>6</v>
@@ -17828,7 +17829,7 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>836</v>
+        <v>880</v>
       </c>
       <c r="B196" t="s">
         <v>6</v>
@@ -17839,7 +17840,7 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>834</v>
+        <v>877</v>
       </c>
       <c r="B197" t="s">
         <v>6</v>
@@ -17850,7 +17851,7 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>830</v>
+        <v>874</v>
       </c>
       <c r="B198" t="s">
         <v>6</v>
@@ -17861,7 +17862,7 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>827</v>
+        <v>871</v>
       </c>
       <c r="B199" t="s">
         <v>6</v>
@@ -17872,7 +17873,7 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>823</v>
+        <v>868</v>
       </c>
       <c r="B200" t="s">
         <v>6</v>
@@ -17883,7 +17884,7 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>820</v>
+        <v>865</v>
       </c>
       <c r="B201" t="s">
         <v>6</v>
@@ -17893,19 +17894,19 @@
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
-        <v>816</v>
+      <c r="A202" s="13" t="s">
+        <v>1395</v>
       </c>
       <c r="B202" t="s">
         <v>6</v>
       </c>
       <c r="C202" t="s">
-        <v>8</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>813</v>
+        <v>862</v>
       </c>
       <c r="B203" t="s">
         <v>6</v>
@@ -17916,7 +17917,7 @@
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>810</v>
+        <v>859</v>
       </c>
       <c r="B204" t="s">
         <v>6</v>
@@ -17927,7 +17928,7 @@
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>808</v>
+        <v>856</v>
       </c>
       <c r="B205" t="s">
         <v>6</v>
@@ -17938,7 +17939,7 @@
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>804</v>
+        <v>853</v>
       </c>
       <c r="B206" t="s">
         <v>6</v>
@@ -17949,7 +17950,7 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>801</v>
+        <v>849</v>
       </c>
       <c r="B207" t="s">
         <v>6</v>
@@ -17960,7 +17961,7 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>798</v>
+        <v>842</v>
       </c>
       <c r="B208" t="s">
         <v>6</v>
@@ -17971,7 +17972,7 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>794</v>
+        <v>845</v>
       </c>
       <c r="B209" t="s">
         <v>6</v>
@@ -17982,7 +17983,7 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>791</v>
+        <v>839</v>
       </c>
       <c r="B210" t="s">
         <v>6</v>
@@ -17993,7 +17994,7 @@
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>788</v>
+        <v>836</v>
       </c>
       <c r="B211" t="s">
         <v>6</v>
@@ -18004,7 +18005,7 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>786</v>
+        <v>834</v>
       </c>
       <c r="B212" t="s">
         <v>6</v>
@@ -18015,7 +18016,7 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>783</v>
+        <v>830</v>
       </c>
       <c r="B213" t="s">
         <v>6</v>
@@ -18026,18 +18027,18 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>780</v>
+        <v>827</v>
       </c>
       <c r="B214" t="s">
         <v>6</v>
       </c>
       <c r="C214" t="s">
-        <v>1392</v>
+        <v>8</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>776</v>
+        <v>823</v>
       </c>
       <c r="B215" t="s">
         <v>6</v>
@@ -18048,7 +18049,7 @@
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>773</v>
+        <v>73</v>
       </c>
       <c r="B216" t="s">
         <v>6</v>
@@ -18059,7 +18060,7 @@
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>770</v>
+        <v>820</v>
       </c>
       <c r="B217" t="s">
         <v>6</v>
@@ -18070,7 +18071,7 @@
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>766</v>
+        <v>94</v>
       </c>
       <c r="B218" t="s">
         <v>6</v>
@@ -18081,7 +18082,7 @@
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>763</v>
+        <v>91</v>
       </c>
       <c r="B219" t="s">
         <v>6</v>
@@ -18092,7 +18093,7 @@
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>760</v>
+        <v>816</v>
       </c>
       <c r="B220" t="s">
         <v>6</v>
@@ -18103,7 +18104,7 @@
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>757</v>
+        <v>813</v>
       </c>
       <c r="B221" t="s">
         <v>6</v>
@@ -18114,7 +18115,7 @@
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>754</v>
+        <v>810</v>
       </c>
       <c r="B222" t="s">
         <v>6</v>
@@ -18125,7 +18126,7 @@
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>752</v>
+        <v>808</v>
       </c>
       <c r="B223" t="s">
         <v>6</v>
@@ -18136,7 +18137,7 @@
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>749</v>
+        <v>804</v>
       </c>
       <c r="B224" t="s">
         <v>6</v>
@@ -18147,7 +18148,7 @@
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>747</v>
+        <v>801</v>
       </c>
       <c r="B225" t="s">
         <v>6</v>
@@ -18158,7 +18159,7 @@
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>744</v>
+        <v>798</v>
       </c>
       <c r="B226" t="s">
         <v>6</v>
@@ -18169,7 +18170,7 @@
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>741</v>
+        <v>794</v>
       </c>
       <c r="B227" t="s">
         <v>6</v>
@@ -18180,7 +18181,7 @@
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>737</v>
+        <v>791</v>
       </c>
       <c r="B228" t="s">
         <v>6</v>
@@ -18191,7 +18192,7 @@
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>734</v>
+        <v>788</v>
       </c>
       <c r="B229" t="s">
         <v>6</v>
@@ -18202,7 +18203,7 @@
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>731</v>
+        <v>786</v>
       </c>
       <c r="B230" t="s">
         <v>6</v>
@@ -18213,7 +18214,7 @@
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>728</v>
+        <v>783</v>
       </c>
       <c r="B231" t="s">
         <v>6</v>
@@ -18224,18 +18225,18 @@
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>725</v>
+        <v>780</v>
       </c>
       <c r="B232" t="s">
         <v>6</v>
       </c>
       <c r="C232" t="s">
-        <v>8</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>722</v>
+        <v>776</v>
       </c>
       <c r="B233" t="s">
         <v>6</v>
@@ -18246,7 +18247,7 @@
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>719</v>
+        <v>773</v>
       </c>
       <c r="B234" t="s">
         <v>6</v>
@@ -18257,7 +18258,7 @@
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>716</v>
+        <v>770</v>
       </c>
       <c r="B235" t="s">
         <v>6</v>
@@ -18268,7 +18269,7 @@
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>712</v>
+        <v>766</v>
       </c>
       <c r="B236" t="s">
         <v>6</v>
@@ -18279,7 +18280,7 @@
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>709</v>
+        <v>763</v>
       </c>
       <c r="B237" t="s">
         <v>6</v>
@@ -18290,7 +18291,7 @@
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>706</v>
+        <v>760</v>
       </c>
       <c r="B238" t="s">
         <v>6</v>
@@ -18301,7 +18302,7 @@
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>703</v>
+        <v>757</v>
       </c>
       <c r="B239" t="s">
         <v>6</v>
@@ -18312,7 +18313,7 @@
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>700</v>
+        <v>754</v>
       </c>
       <c r="B240" t="s">
         <v>6</v>
@@ -18323,7 +18324,7 @@
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>697</v>
+        <v>749</v>
       </c>
       <c r="B241" t="s">
         <v>6</v>
@@ -18334,7 +18335,7 @@
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>695</v>
+        <v>752</v>
       </c>
       <c r="B242" t="s">
         <v>6</v>
@@ -18345,7 +18346,7 @@
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>692</v>
+        <v>747</v>
       </c>
       <c r="B243" t="s">
         <v>6</v>
@@ -18356,7 +18357,7 @@
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>689</v>
+        <v>744</v>
       </c>
       <c r="B244" t="s">
         <v>6</v>
@@ -18367,7 +18368,7 @@
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>686</v>
+        <v>741</v>
       </c>
       <c r="B245" t="s">
         <v>6</v>
@@ -18378,7 +18379,7 @@
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>682</v>
+        <v>737</v>
       </c>
       <c r="B246" t="s">
         <v>6</v>
@@ -18389,7 +18390,7 @@
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>679</v>
+        <v>734</v>
       </c>
       <c r="B247" t="s">
         <v>6</v>
@@ -18400,7 +18401,7 @@
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>676</v>
+        <v>731</v>
       </c>
       <c r="B248" t="s">
         <v>6</v>
@@ -18411,7 +18412,7 @@
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>673</v>
+        <v>728</v>
       </c>
       <c r="B249" t="s">
         <v>6</v>
@@ -18422,7 +18423,7 @@
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>670</v>
+        <v>725</v>
       </c>
       <c r="B250" t="s">
         <v>6</v>
@@ -18433,7 +18434,7 @@
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>668</v>
+        <v>722</v>
       </c>
       <c r="B251" t="s">
         <v>6</v>
@@ -18444,18 +18445,18 @@
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>665</v>
+        <v>719</v>
       </c>
       <c r="B252" t="s">
         <v>6</v>
       </c>
       <c r="C252" t="s">
-        <v>1392</v>
+        <v>8</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>662</v>
+        <v>716</v>
       </c>
       <c r="B253" t="s">
         <v>6</v>
@@ -18466,7 +18467,7 @@
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>660</v>
+        <v>89</v>
       </c>
       <c r="B254" t="s">
         <v>6</v>
@@ -18477,7 +18478,7 @@
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>657</v>
+        <v>712</v>
       </c>
       <c r="B255" t="s">
         <v>6</v>
@@ -18488,7 +18489,7 @@
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>655</v>
+        <v>709</v>
       </c>
       <c r="B256" t="s">
         <v>6</v>
@@ -18499,7 +18500,7 @@
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>652</v>
+        <v>706</v>
       </c>
       <c r="B257" t="s">
         <v>6</v>
@@ -18510,7 +18511,7 @@
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>649</v>
+        <v>703</v>
       </c>
       <c r="B258" t="s">
         <v>6</v>
@@ -18521,7 +18522,7 @@
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>646</v>
+        <v>700</v>
       </c>
       <c r="B259" t="s">
         <v>6</v>
@@ -18532,7 +18533,7 @@
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>642</v>
+        <v>697</v>
       </c>
       <c r="B260" t="s">
         <v>6</v>
@@ -18543,7 +18544,7 @@
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>639</v>
+        <v>695</v>
       </c>
       <c r="B261" t="s">
         <v>6</v>
@@ -18554,7 +18555,7 @@
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>636</v>
+        <v>692</v>
       </c>
       <c r="B262" t="s">
         <v>6</v>
@@ -18565,7 +18566,7 @@
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>633</v>
+        <v>689</v>
       </c>
       <c r="B263" t="s">
         <v>6</v>
@@ -18576,7 +18577,7 @@
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>630</v>
+        <v>686</v>
       </c>
       <c r="B264" t="s">
         <v>6</v>
@@ -18587,7 +18588,7 @@
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>627</v>
+        <v>682</v>
       </c>
       <c r="B265" t="s">
         <v>6</v>
@@ -18598,7 +18599,7 @@
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>624</v>
+        <v>679</v>
       </c>
       <c r="B266" t="s">
         <v>6</v>
@@ -18609,7 +18610,7 @@
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>621</v>
+        <v>676</v>
       </c>
       <c r="B267" t="s">
         <v>6</v>
@@ -18620,7 +18621,7 @@
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>618</v>
+        <v>673</v>
       </c>
       <c r="B268" t="s">
         <v>6</v>
@@ -18631,7 +18632,7 @@
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>615</v>
+        <v>670</v>
       </c>
       <c r="B269" t="s">
         <v>6</v>
@@ -18642,7 +18643,7 @@
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>612</v>
+        <v>668</v>
       </c>
       <c r="B270" t="s">
         <v>6</v>
@@ -18653,29 +18654,29 @@
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>609</v>
+        <v>665</v>
       </c>
       <c r="B271" t="s">
         <v>6</v>
       </c>
       <c r="C271" t="s">
-        <v>8</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>606</v>
+        <v>662</v>
       </c>
       <c r="B272" t="s">
         <v>6</v>
       </c>
       <c r="C272" t="s">
-        <v>1392</v>
+        <v>8</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>602</v>
+        <v>660</v>
       </c>
       <c r="B273" t="s">
         <v>6</v>
@@ -18686,7 +18687,7 @@
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>598</v>
+        <v>657</v>
       </c>
       <c r="B274" t="s">
         <v>6</v>
@@ -18697,7 +18698,7 @@
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>595</v>
+        <v>655</v>
       </c>
       <c r="B275" t="s">
         <v>6</v>
@@ -18708,7 +18709,7 @@
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>593</v>
+        <v>652</v>
       </c>
       <c r="B276" t="s">
         <v>6</v>
@@ -18719,7 +18720,7 @@
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>591</v>
+        <v>649</v>
       </c>
       <c r="B277" t="s">
         <v>6</v>
@@ -18730,7 +18731,7 @@
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>588</v>
+        <v>646</v>
       </c>
       <c r="B278" t="s">
         <v>6</v>
@@ -18741,18 +18742,18 @@
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>585</v>
+        <v>642</v>
       </c>
       <c r="B279" t="s">
         <v>6</v>
       </c>
       <c r="C279" t="s">
-        <v>1392</v>
+        <v>8</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>581</v>
+        <v>639</v>
       </c>
       <c r="B280" t="s">
         <v>6</v>
@@ -18763,7 +18764,7 @@
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>578</v>
+        <v>636</v>
       </c>
       <c r="B281" t="s">
         <v>6</v>
@@ -18774,7 +18775,7 @@
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>576</v>
+        <v>633</v>
       </c>
       <c r="B282" t="s">
         <v>6</v>
@@ -18785,7 +18786,7 @@
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>572</v>
+        <v>630</v>
       </c>
       <c r="B283" t="s">
         <v>6</v>
@@ -18796,7 +18797,7 @@
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>570</v>
+        <v>627</v>
       </c>
       <c r="B284" t="s">
         <v>6</v>
@@ -18807,7 +18808,7 @@
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>567</v>
+        <v>624</v>
       </c>
       <c r="B285" t="s">
         <v>6</v>
@@ -18818,7 +18819,7 @@
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>563</v>
+        <v>621</v>
       </c>
       <c r="B286" t="s">
         <v>6</v>
@@ -18829,7 +18830,7 @@
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>560</v>
+        <v>618</v>
       </c>
       <c r="B287" t="s">
         <v>6</v>
@@ -18840,7 +18841,7 @@
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>557</v>
+        <v>615</v>
       </c>
       <c r="B288" t="s">
         <v>6</v>
@@ -18851,18 +18852,18 @@
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>554</v>
+        <v>58</v>
       </c>
       <c r="B289" t="s">
         <v>6</v>
       </c>
       <c r="C289" t="s">
-        <v>8</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>551</v>
+        <v>612</v>
       </c>
       <c r="B290" t="s">
         <v>6</v>
@@ -18873,7 +18874,7 @@
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>447</v>
+        <v>609</v>
       </c>
       <c r="B291" t="s">
         <v>6</v>
@@ -18884,18 +18885,18 @@
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>546</v>
+        <v>606</v>
       </c>
       <c r="B292" t="s">
         <v>6</v>
       </c>
       <c r="C292" t="s">
-        <v>8</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>543</v>
+        <v>602</v>
       </c>
       <c r="B293" t="s">
         <v>6</v>
@@ -18906,7 +18907,7 @@
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>540</v>
+        <v>598</v>
       </c>
       <c r="B294" t="s">
         <v>6</v>
@@ -18917,7 +18918,7 @@
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>537</v>
+        <v>595</v>
       </c>
       <c r="B295" t="s">
         <v>6</v>
@@ -18928,7 +18929,7 @@
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>534</v>
+        <v>593</v>
       </c>
       <c r="B296" t="s">
         <v>6</v>
@@ -18939,7 +18940,7 @@
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>532</v>
+        <v>591</v>
       </c>
       <c r="B297" t="s">
         <v>6</v>
@@ -18950,7 +18951,7 @@
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>528</v>
+        <v>588</v>
       </c>
       <c r="B298" t="s">
         <v>6</v>
@@ -18961,18 +18962,18 @@
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>525</v>
+        <v>585</v>
       </c>
       <c r="B299" t="s">
         <v>6</v>
       </c>
       <c r="C299" t="s">
-        <v>8</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>522</v>
+        <v>56</v>
       </c>
       <c r="B300" t="s">
         <v>6</v>
@@ -18983,7 +18984,7 @@
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>519</v>
+        <v>53</v>
       </c>
       <c r="B301" t="s">
         <v>6</v>
@@ -18994,7 +18995,7 @@
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>516</v>
+        <v>581</v>
       </c>
       <c r="B302" t="s">
         <v>6</v>
@@ -19005,7 +19006,7 @@
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>513</v>
+        <v>578</v>
       </c>
       <c r="B303" t="s">
         <v>6</v>
@@ -19016,7 +19017,7 @@
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>510</v>
+        <v>576</v>
       </c>
       <c r="B304" t="s">
         <v>6</v>
@@ -19027,7 +19028,7 @@
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>507</v>
+        <v>572</v>
       </c>
       <c r="B305" t="s">
         <v>6</v>
@@ -19038,7 +19039,7 @@
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>504</v>
+        <v>570</v>
       </c>
       <c r="B306" t="s">
         <v>6</v>
@@ -19049,7 +19050,7 @@
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>501</v>
+        <v>567</v>
       </c>
       <c r="B307" t="s">
         <v>6</v>
@@ -19060,7 +19061,7 @@
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>498</v>
+        <v>563</v>
       </c>
       <c r="B308" t="s">
         <v>6</v>
@@ -19071,7 +19072,7 @@
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>495</v>
+        <v>560</v>
       </c>
       <c r="B309" t="s">
         <v>6</v>
@@ -19082,7 +19083,7 @@
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>492</v>
+        <v>557</v>
       </c>
       <c r="B310" t="s">
         <v>6</v>
@@ -19093,7 +19094,7 @@
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>491</v>
+        <v>554</v>
       </c>
       <c r="B311" t="s">
         <v>6</v>
@@ -19103,8 +19104,8 @@
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A312" t="s">
-        <v>489</v>
+      <c r="A312" s="13" t="s">
+        <v>38</v>
       </c>
       <c r="B312" t="s">
         <v>6</v>
@@ -19115,7 +19116,7 @@
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>486</v>
+        <v>551</v>
       </c>
       <c r="B313" t="s">
         <v>6</v>
@@ -19126,7 +19127,7 @@
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>483</v>
+        <v>447</v>
       </c>
       <c r="B314" t="s">
         <v>6</v>
@@ -19137,18 +19138,18 @@
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>479</v>
+        <v>546</v>
       </c>
       <c r="B315" t="s">
         <v>6</v>
       </c>
       <c r="C315" t="s">
-        <v>1392</v>
+        <v>8</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>475</v>
+        <v>543</v>
       </c>
       <c r="B316" t="s">
         <v>6</v>
@@ -19159,7 +19160,7 @@
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>472</v>
+        <v>540</v>
       </c>
       <c r="B317" t="s">
         <v>6</v>
@@ -19170,7 +19171,7 @@
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>469</v>
+        <v>537</v>
       </c>
       <c r="B318" t="s">
         <v>6</v>
@@ -19181,7 +19182,7 @@
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>466</v>
+        <v>534</v>
       </c>
       <c r="B319" t="s">
         <v>6</v>
@@ -19192,7 +19193,7 @@
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>463</v>
+        <v>69</v>
       </c>
       <c r="B320" t="s">
         <v>6</v>
@@ -19202,8 +19203,8 @@
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A321" t="s">
-        <v>460</v>
+      <c r="A321" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="B321" t="s">
         <v>6</v>
@@ -19214,7 +19215,7 @@
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>457</v>
+        <v>99</v>
       </c>
       <c r="B322" t="s">
         <v>6</v>
@@ -19225,7 +19226,7 @@
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>454</v>
+        <v>532</v>
       </c>
       <c r="B323" t="s">
         <v>6</v>
@@ -19236,7 +19237,7 @@
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>451</v>
+        <v>528</v>
       </c>
       <c r="B324" t="s">
         <v>6</v>
@@ -19247,7 +19248,7 @@
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>448</v>
+        <v>525</v>
       </c>
       <c r="B325" t="s">
         <v>6</v>
@@ -19258,7 +19259,7 @@
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
-        <v>445</v>
+        <v>522</v>
       </c>
       <c r="B326" t="s">
         <v>6</v>
@@ -19269,7 +19270,7 @@
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>443</v>
+        <v>96</v>
       </c>
       <c r="B327" t="s">
         <v>6</v>
@@ -19280,7 +19281,7 @@
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
-        <v>440</v>
+        <v>67</v>
       </c>
       <c r="B328" t="s">
         <v>6</v>
@@ -19291,7 +19292,7 @@
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
-        <v>437</v>
+        <v>65</v>
       </c>
       <c r="B329" t="s">
         <v>6</v>
@@ -19302,7 +19303,7 @@
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
-        <v>434</v>
+        <v>519</v>
       </c>
       <c r="B330" t="s">
         <v>6</v>
@@ -19313,7 +19314,7 @@
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>431</v>
+        <v>516</v>
       </c>
       <c r="B331" t="s">
         <v>6</v>
@@ -19324,7 +19325,7 @@
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>428</v>
+        <v>513</v>
       </c>
       <c r="B332" t="s">
         <v>6</v>
@@ -19335,7 +19336,7 @@
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>425</v>
+        <v>510</v>
       </c>
       <c r="B333" t="s">
         <v>6</v>
@@ -19346,7 +19347,7 @@
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>422</v>
+        <v>507</v>
       </c>
       <c r="B334" t="s">
         <v>6</v>
@@ -19357,7 +19358,7 @@
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>418</v>
+        <v>504</v>
       </c>
       <c r="B335" t="s">
         <v>6</v>
@@ -19368,7 +19369,7 @@
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>415</v>
+        <v>501</v>
       </c>
       <c r="B336" t="s">
         <v>6</v>
@@ -19379,7 +19380,7 @@
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>411</v>
+        <v>498</v>
       </c>
       <c r="B337" t="s">
         <v>6</v>
@@ -19390,7 +19391,7 @@
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>408</v>
+        <v>495</v>
       </c>
       <c r="B338" t="s">
         <v>6</v>
@@ -19401,7 +19402,7 @@
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>405</v>
+        <v>492</v>
       </c>
       <c r="B339" t="s">
         <v>6</v>
@@ -19412,7 +19413,7 @@
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>402</v>
+        <v>486</v>
       </c>
       <c r="B340" t="s">
         <v>6</v>
@@ -19423,7 +19424,7 @@
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>400</v>
+        <v>489</v>
       </c>
       <c r="B341" t="s">
         <v>6</v>
@@ -19434,7 +19435,7 @@
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>397</v>
+        <v>491</v>
       </c>
       <c r="B342" t="s">
         <v>6</v>
@@ -19445,7 +19446,7 @@
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>394</v>
+        <v>483</v>
       </c>
       <c r="B343" t="s">
         <v>6</v>
@@ -19456,18 +19457,18 @@
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>391</v>
+        <v>479</v>
       </c>
       <c r="B344" t="s">
         <v>6</v>
       </c>
       <c r="C344" t="s">
-        <v>8</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>388</v>
+        <v>475</v>
       </c>
       <c r="B345" t="s">
         <v>6</v>
@@ -19478,7 +19479,7 @@
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>385</v>
+        <v>472</v>
       </c>
       <c r="B346" t="s">
         <v>6</v>
@@ -19489,7 +19490,7 @@
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>382</v>
+        <v>469</v>
       </c>
       <c r="B347" t="s">
         <v>6</v>
@@ -19500,7 +19501,7 @@
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>379</v>
+        <v>466</v>
       </c>
       <c r="B348" t="s">
         <v>6</v>
@@ -19511,7 +19512,7 @@
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>375</v>
+        <v>463</v>
       </c>
       <c r="B349" t="s">
         <v>6</v>
@@ -19522,7 +19523,7 @@
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>372</v>
+        <v>460</v>
       </c>
       <c r="B350" t="s">
         <v>6</v>
@@ -19533,7 +19534,7 @@
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>370</v>
+        <v>457</v>
       </c>
       <c r="B351" t="s">
         <v>6</v>
@@ -19544,7 +19545,7 @@
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
-        <v>368</v>
+        <v>454</v>
       </c>
       <c r="B352" t="s">
         <v>6</v>
@@ -19555,7 +19556,7 @@
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>366</v>
+        <v>451</v>
       </c>
       <c r="B353" t="s">
         <v>6</v>
@@ -19566,7 +19567,7 @@
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>363</v>
+        <v>448</v>
       </c>
       <c r="B354" t="s">
         <v>6</v>
@@ -19577,7 +19578,7 @@
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>361</v>
+        <v>445</v>
       </c>
       <c r="B355" t="s">
         <v>6</v>
@@ -19588,7 +19589,7 @@
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>358</v>
+        <v>443</v>
       </c>
       <c r="B356" t="s">
         <v>6</v>
@@ -19599,7 +19600,7 @@
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>356</v>
+        <v>440</v>
       </c>
       <c r="B357" t="s">
         <v>6</v>
@@ -19610,7 +19611,7 @@
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>353</v>
+        <v>437</v>
       </c>
       <c r="B358" t="s">
         <v>6</v>
@@ -19621,7 +19622,7 @@
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>350</v>
+        <v>434</v>
       </c>
       <c r="B359" t="s">
         <v>6</v>
@@ -19632,7 +19633,7 @@
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>347</v>
+        <v>431</v>
       </c>
       <c r="B360" t="s">
         <v>6</v>
@@ -19643,7 +19644,7 @@
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>344</v>
+        <v>428</v>
       </c>
       <c r="B361" t="s">
         <v>6</v>
@@ -19654,7 +19655,7 @@
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>341</v>
+        <v>425</v>
       </c>
       <c r="B362" t="s">
         <v>6</v>
@@ -19665,7 +19666,7 @@
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>340</v>
+        <v>422</v>
       </c>
       <c r="B363" t="s">
         <v>6</v>
@@ -19676,7 +19677,7 @@
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>337</v>
+        <v>418</v>
       </c>
       <c r="B364" t="s">
         <v>6</v>
@@ -19687,7 +19688,7 @@
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>335</v>
+        <v>415</v>
       </c>
       <c r="B365" t="s">
         <v>6</v>
@@ -19698,7 +19699,7 @@
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>332</v>
+        <v>411</v>
       </c>
       <c r="B366" t="s">
         <v>6</v>
@@ -19709,7 +19710,7 @@
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>329</v>
+        <v>408</v>
       </c>
       <c r="B367" t="s">
         <v>6</v>
@@ -19720,7 +19721,7 @@
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>327</v>
+        <v>405</v>
       </c>
       <c r="B368" t="s">
         <v>6</v>
@@ -19731,7 +19732,7 @@
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>324</v>
+        <v>402</v>
       </c>
       <c r="B369" t="s">
         <v>6</v>
@@ -19742,7 +19743,7 @@
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>321</v>
+        <v>400</v>
       </c>
       <c r="B370" t="s">
         <v>6</v>
@@ -19753,7 +19754,7 @@
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>318</v>
+        <v>397</v>
       </c>
       <c r="B371" t="s">
         <v>6</v>
@@ -19764,7 +19765,7 @@
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>313</v>
+        <v>394</v>
       </c>
       <c r="B372" t="s">
         <v>6</v>
@@ -19775,7 +19776,7 @@
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>311</v>
+        <v>391</v>
       </c>
       <c r="B373" t="s">
         <v>6</v>
@@ -19786,7 +19787,7 @@
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>308</v>
+        <v>388</v>
       </c>
       <c r="B374" t="s">
         <v>6</v>
@@ -19797,7 +19798,7 @@
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>306</v>
+        <v>385</v>
       </c>
       <c r="B375" t="s">
         <v>6</v>
@@ -19808,7 +19809,7 @@
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>303</v>
+        <v>382</v>
       </c>
       <c r="B376" t="s">
         <v>6</v>
@@ -19819,7 +19820,7 @@
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>300</v>
+        <v>379</v>
       </c>
       <c r="B377" t="s">
         <v>6</v>
@@ -19830,7 +19831,7 @@
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>297</v>
+        <v>375</v>
       </c>
       <c r="B378" t="s">
         <v>6</v>
@@ -19841,7 +19842,7 @@
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
-        <v>295</v>
+        <v>372</v>
       </c>
       <c r="B379" t="s">
         <v>6</v>
@@ -19852,18 +19853,18 @@
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
-        <v>291</v>
+        <v>55</v>
       </c>
       <c r="B380" t="s">
         <v>6</v>
       </c>
       <c r="C380" t="s">
-        <v>8</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>289</v>
+        <v>370</v>
       </c>
       <c r="B381" t="s">
         <v>6</v>
@@ -19873,8 +19874,8 @@
       </c>
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A382" t="s">
-        <v>287</v>
+      <c r="A382" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="B382" t="s">
         <v>6</v>
@@ -19885,7 +19886,7 @@
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
-        <v>284</v>
+        <v>368</v>
       </c>
       <c r="B383" t="s">
         <v>6</v>
@@ -19896,7 +19897,7 @@
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
-        <v>281</v>
+        <v>363</v>
       </c>
       <c r="B384" t="s">
         <v>6</v>
@@ -19907,7 +19908,7 @@
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
-        <v>278</v>
+        <v>366</v>
       </c>
       <c r="B385" t="s">
         <v>6</v>
@@ -19918,7 +19919,7 @@
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
-        <v>275</v>
+        <v>361</v>
       </c>
       <c r="B386" t="s">
         <v>6</v>
@@ -19929,7 +19930,7 @@
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
-        <v>271</v>
+        <v>358</v>
       </c>
       <c r="B387" t="s">
         <v>6</v>
@@ -19940,7 +19941,7 @@
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
-        <v>268</v>
+        <v>356</v>
       </c>
       <c r="B388" t="s">
         <v>6</v>
@@ -19951,7 +19952,7 @@
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>265</v>
+        <v>353</v>
       </c>
       <c r="B389" t="s">
         <v>6</v>
@@ -19962,7 +19963,7 @@
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
-        <v>263</v>
+        <v>350</v>
       </c>
       <c r="B390" t="s">
         <v>6</v>
@@ -19973,7 +19974,7 @@
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
-        <v>260</v>
+        <v>87</v>
       </c>
       <c r="B391" t="s">
         <v>6</v>
@@ -19983,8 +19984,8 @@
       </c>
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A392" t="s">
-        <v>258</v>
+      <c r="A392" s="13" t="s">
+        <v>43</v>
       </c>
       <c r="B392" t="s">
         <v>6</v>
@@ -19995,7 +19996,7 @@
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
-        <v>255</v>
+        <v>347</v>
       </c>
       <c r="B393" t="s">
         <v>6</v>
@@ -20006,7 +20007,7 @@
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
-        <v>252</v>
+        <v>71</v>
       </c>
       <c r="B394" t="s">
         <v>6</v>
@@ -20017,7 +20018,7 @@
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
-        <v>249</v>
+        <v>344</v>
       </c>
       <c r="B395" t="s">
         <v>6</v>
@@ -20028,7 +20029,7 @@
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
-        <v>246</v>
+        <v>341</v>
       </c>
       <c r="B396" t="s">
         <v>6</v>
@@ -20039,7 +20040,7 @@
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
-        <v>243</v>
+        <v>340</v>
       </c>
       <c r="B397" t="s">
         <v>6</v>
@@ -20050,7 +20051,7 @@
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
-        <v>240</v>
+        <v>337</v>
       </c>
       <c r="B398" t="s">
         <v>6</v>
@@ -20061,7 +20062,7 @@
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
-        <v>237</v>
+        <v>335</v>
       </c>
       <c r="B399" t="s">
         <v>6</v>
@@ -20072,7 +20073,7 @@
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
-        <v>234</v>
+        <v>332</v>
       </c>
       <c r="B400" t="s">
         <v>6</v>
@@ -20083,7 +20084,7 @@
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
-        <v>231</v>
+        <v>329</v>
       </c>
       <c r="B401" t="s">
         <v>6</v>
@@ -20094,7 +20095,7 @@
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
-        <v>228</v>
+        <v>327</v>
       </c>
       <c r="B402" t="s">
         <v>6</v>
@@ -20105,7 +20106,7 @@
     </row>
     <row r="403" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
-        <v>225</v>
+        <v>324</v>
       </c>
       <c r="B403" t="s">
         <v>6</v>
@@ -20116,7 +20117,7 @@
     </row>
     <row r="404" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
-        <v>221</v>
+        <v>321</v>
       </c>
       <c r="B404" t="s">
         <v>6</v>
@@ -20127,7 +20128,7 @@
     </row>
     <row r="405" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
-        <v>218</v>
+        <v>318</v>
       </c>
       <c r="B405" t="s">
         <v>6</v>
@@ -20138,7 +20139,7 @@
     </row>
     <row r="406" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
-        <v>215</v>
+        <v>313</v>
       </c>
       <c r="B406" t="s">
         <v>6</v>
@@ -20149,7 +20150,7 @@
     </row>
     <row r="407" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
-        <v>212</v>
+        <v>311</v>
       </c>
       <c r="B407" t="s">
         <v>6</v>
@@ -20160,7 +20161,7 @@
     </row>
     <row r="408" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
-        <v>209</v>
+        <v>308</v>
       </c>
       <c r="B408" t="s">
         <v>6</v>
@@ -20171,7 +20172,7 @@
     </row>
     <row r="409" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
-        <v>206</v>
+        <v>306</v>
       </c>
       <c r="B409" t="s">
         <v>6</v>
@@ -20182,7 +20183,7 @@
     </row>
     <row r="410" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
-        <v>203</v>
+        <v>303</v>
       </c>
       <c r="B410" t="s">
         <v>6</v>
@@ -20193,7 +20194,7 @@
     </row>
     <row r="411" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="B411" t="s">
         <v>6</v>
@@ -20204,7 +20205,7 @@
     </row>
     <row r="412" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
-        <v>197</v>
+        <v>297</v>
       </c>
       <c r="B412" t="s">
         <v>6</v>
@@ -20215,7 +20216,7 @@
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
-        <v>194</v>
+        <v>295</v>
       </c>
       <c r="B413" t="s">
         <v>6</v>
@@ -20226,7 +20227,7 @@
     </row>
     <row r="414" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
-        <v>191</v>
+        <v>291</v>
       </c>
       <c r="B414" t="s">
         <v>6</v>
@@ -20237,7 +20238,7 @@
     </row>
     <row r="415" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
-        <v>188</v>
+        <v>289</v>
       </c>
       <c r="B415" t="s">
         <v>6</v>
@@ -20248,7 +20249,7 @@
     </row>
     <row r="416" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
-        <v>184</v>
+        <v>287</v>
       </c>
       <c r="B416" t="s">
         <v>6</v>
@@ -20259,7 +20260,7 @@
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
-        <v>181</v>
+        <v>284</v>
       </c>
       <c r="B417" t="s">
         <v>6</v>
@@ -20270,7 +20271,7 @@
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
-        <v>178</v>
+        <v>281</v>
       </c>
       <c r="B418" t="s">
         <v>6</v>
@@ -20281,7 +20282,7 @@
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
-        <v>175</v>
+        <v>278</v>
       </c>
       <c r="B419" t="s">
         <v>6</v>
@@ -20292,7 +20293,7 @@
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
-        <v>172</v>
+        <v>275</v>
       </c>
       <c r="B420" t="s">
         <v>6</v>
@@ -20303,7 +20304,7 @@
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
-        <v>169</v>
+        <v>265</v>
       </c>
       <c r="B421" t="s">
         <v>6</v>
@@ -20314,7 +20315,7 @@
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
-        <v>166</v>
+        <v>271</v>
       </c>
       <c r="B422" t="s">
         <v>6</v>
@@ -20325,7 +20326,7 @@
     </row>
     <row r="423" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
-        <v>163</v>
+        <v>268</v>
       </c>
       <c r="B423" t="s">
         <v>6</v>
@@ -20336,7 +20337,7 @@
     </row>
     <row r="424" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
-        <v>160</v>
+        <v>263</v>
       </c>
       <c r="B424" t="s">
         <v>6</v>
@@ -20347,7 +20348,7 @@
     </row>
     <row r="425" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
-        <v>157</v>
+        <v>260</v>
       </c>
       <c r="B425" t="s">
         <v>6</v>
@@ -20358,7 +20359,7 @@
     </row>
     <row r="426" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
-        <v>154</v>
+        <v>258</v>
       </c>
       <c r="B426" t="s">
         <v>6</v>
@@ -20369,7 +20370,7 @@
     </row>
     <row r="427" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
-        <v>151</v>
+        <v>255</v>
       </c>
       <c r="B427" t="s">
         <v>6</v>
@@ -20380,7 +20381,7 @@
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
-        <v>148</v>
+        <v>252</v>
       </c>
       <c r="B428" t="s">
         <v>6</v>
@@ -20391,7 +20392,7 @@
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
-        <v>144</v>
+        <v>249</v>
       </c>
       <c r="B429" t="s">
         <v>6</v>
@@ -20402,7 +20403,7 @@
     </row>
     <row r="430" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
-        <v>141</v>
+        <v>246</v>
       </c>
       <c r="B430" t="s">
         <v>6</v>
@@ -20413,7 +20414,7 @@
     </row>
     <row r="431" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
-        <v>138</v>
+        <v>243</v>
       </c>
       <c r="B431" t="s">
         <v>6</v>
@@ -20424,18 +20425,18 @@
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
-        <v>135</v>
+        <v>240</v>
       </c>
       <c r="B432" t="s">
         <v>6</v>
       </c>
       <c r="C432" t="s">
-        <v>1392</v>
+        <v>8</v>
       </c>
     </row>
     <row r="433" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
-        <v>131</v>
+        <v>237</v>
       </c>
       <c r="B433" t="s">
         <v>6</v>
@@ -20446,7 +20447,7 @@
     </row>
     <row r="434" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
-        <v>128</v>
+        <v>234</v>
       </c>
       <c r="B434" t="s">
         <v>6</v>
@@ -20457,7 +20458,7 @@
     </row>
     <row r="435" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
-        <v>125</v>
+        <v>231</v>
       </c>
       <c r="B435" t="s">
         <v>6</v>
@@ -20468,7 +20469,7 @@
     </row>
     <row r="436" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
-        <v>122</v>
+        <v>228</v>
       </c>
       <c r="B436" t="s">
         <v>6</v>
@@ -20479,7 +20480,7 @@
     </row>
     <row r="437" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
-        <v>119</v>
+        <v>225</v>
       </c>
       <c r="B437" t="s">
         <v>6</v>
@@ -20490,7 +20491,7 @@
     </row>
     <row r="438" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
-        <v>116</v>
+        <v>221</v>
       </c>
       <c r="B438" t="s">
         <v>6</v>
@@ -20501,7 +20502,7 @@
     </row>
     <row r="439" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
-        <v>113</v>
+        <v>218</v>
       </c>
       <c r="B439" t="s">
         <v>6</v>
@@ -20512,7 +20513,7 @@
     </row>
     <row r="440" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
-        <v>110</v>
+        <v>215</v>
       </c>
       <c r="B440" t="s">
         <v>6</v>
@@ -20523,7 +20524,7 @@
     </row>
     <row r="441" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
-        <v>106</v>
+        <v>212</v>
       </c>
       <c r="B441" t="s">
         <v>6</v>
@@ -20534,7 +20535,7 @@
     </row>
     <row r="442" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
-        <v>103</v>
+        <v>209</v>
       </c>
       <c r="B442" t="s">
         <v>6</v>
@@ -20545,7 +20546,7 @@
     </row>
     <row r="443" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
-        <v>102</v>
+        <v>206</v>
       </c>
       <c r="B443" t="s">
         <v>6</v>
@@ -20556,18 +20557,18 @@
     </row>
     <row r="444" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
-        <v>99</v>
+        <v>54</v>
       </c>
       <c r="B444" t="s">
         <v>6</v>
       </c>
       <c r="C444" t="s">
-        <v>8</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="445" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
-        <v>96</v>
+        <v>203</v>
       </c>
       <c r="B445" t="s">
         <v>6</v>
@@ -20578,7 +20579,7 @@
     </row>
     <row r="446" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
-        <v>94</v>
+        <v>200</v>
       </c>
       <c r="B446" t="s">
         <v>6</v>
@@ -20589,7 +20590,7 @@
     </row>
     <row r="447" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
-        <v>91</v>
+        <v>197</v>
       </c>
       <c r="B447" t="s">
         <v>6</v>
@@ -20600,7 +20601,7 @@
     </row>
     <row r="448" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
-        <v>89</v>
+        <v>194</v>
       </c>
       <c r="B448" t="s">
         <v>6</v>
@@ -20611,7 +20612,7 @@
     </row>
     <row r="449" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
-        <v>87</v>
+        <v>191</v>
       </c>
       <c r="B449" t="s">
         <v>6</v>
@@ -20622,7 +20623,7 @@
     </row>
     <row r="450" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
-        <v>85</v>
+        <v>188</v>
       </c>
       <c r="B450" t="s">
         <v>6</v>
@@ -20633,7 +20634,7 @@
     </row>
     <row r="451" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
-        <v>83</v>
+        <v>184</v>
       </c>
       <c r="B451" t="s">
         <v>6</v>
@@ -20644,7 +20645,7 @@
     </row>
     <row r="452" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
-        <v>81</v>
+        <v>181</v>
       </c>
       <c r="B452" t="s">
         <v>6</v>
@@ -20655,7 +20656,7 @@
     </row>
     <row r="453" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
-        <v>79</v>
+        <v>178</v>
       </c>
       <c r="B453" t="s">
         <v>6</v>
@@ -20666,7 +20667,7 @@
     </row>
     <row r="454" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
-        <v>77</v>
+        <v>175</v>
       </c>
       <c r="B454" t="s">
         <v>6</v>
@@ -20677,7 +20678,7 @@
     </row>
     <row r="455" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
-        <v>75</v>
+        <v>172</v>
       </c>
       <c r="B455" t="s">
         <v>6</v>
@@ -20688,7 +20689,7 @@
     </row>
     <row r="456" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
-        <v>73</v>
+        <v>169</v>
       </c>
       <c r="B456" t="s">
         <v>6</v>
@@ -20699,7 +20700,7 @@
     </row>
     <row r="457" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
-        <v>71</v>
+        <v>166</v>
       </c>
       <c r="B457" t="s">
         <v>6</v>
@@ -20710,7 +20711,7 @@
     </row>
     <row r="458" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
-        <v>69</v>
+        <v>163</v>
       </c>
       <c r="B458" t="s">
         <v>6</v>
@@ -20721,7 +20722,7 @@
     </row>
     <row r="459" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
-        <v>67</v>
+        <v>160</v>
       </c>
       <c r="B459" t="s">
         <v>6</v>
@@ -20732,7 +20733,7 @@
     </row>
     <row r="460" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
-        <v>65</v>
+        <v>157</v>
       </c>
       <c r="B460" t="s">
         <v>6</v>
@@ -20743,7 +20744,7 @@
     </row>
     <row r="461" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
-        <v>63</v>
+        <v>154</v>
       </c>
       <c r="B461" t="s">
         <v>6</v>
@@ -20754,7 +20755,7 @@
     </row>
     <row r="462" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
-        <v>62</v>
+        <v>151</v>
       </c>
       <c r="B462" t="s">
         <v>6</v>
@@ -20765,7 +20766,7 @@
     </row>
     <row r="463" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
-        <v>61</v>
+        <v>148</v>
       </c>
       <c r="B463" t="s">
         <v>6</v>
@@ -20776,7 +20777,7 @@
     </row>
     <row r="464" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
-        <v>60</v>
+        <v>144</v>
       </c>
       <c r="B464" t="s">
         <v>6</v>
@@ -20787,62 +20788,62 @@
     </row>
     <row r="465" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
-        <v>59</v>
+        <v>141</v>
       </c>
       <c r="B465" t="s">
         <v>6</v>
       </c>
       <c r="C465" t="s">
-        <v>1393</v>
+        <v>8</v>
       </c>
     </row>
     <row r="466" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
-        <v>58</v>
+        <v>138</v>
       </c>
       <c r="B466" t="s">
         <v>6</v>
       </c>
       <c r="C466" t="s">
-        <v>1392</v>
+        <v>8</v>
       </c>
     </row>
     <row r="467" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
-        <v>56</v>
+        <v>135</v>
       </c>
       <c r="B467" t="s">
         <v>6</v>
       </c>
       <c r="C467" t="s">
-        <v>8</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="468" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
-        <v>55</v>
+        <v>131</v>
       </c>
       <c r="B468" t="s">
         <v>6</v>
       </c>
       <c r="C468" t="s">
-        <v>1392</v>
+        <v>8</v>
       </c>
     </row>
     <row r="469" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
-        <v>54</v>
+        <v>128</v>
       </c>
       <c r="B469" t="s">
         <v>6</v>
       </c>
       <c r="C469" t="s">
-        <v>1392</v>
+        <v>8</v>
       </c>
     </row>
     <row r="470" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
-        <v>53</v>
+        <v>125</v>
       </c>
       <c r="B470" t="s">
         <v>6</v>
@@ -20853,7 +20854,7 @@
     </row>
     <row r="471" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
-        <v>52</v>
+        <v>122</v>
       </c>
       <c r="B471" t="s">
         <v>6</v>
@@ -20863,8 +20864,8 @@
       </c>
     </row>
     <row r="472" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A472" s="13" t="s">
-        <v>51</v>
+      <c r="A472" t="s">
+        <v>119</v>
       </c>
       <c r="B472" t="s">
         <v>6</v>
@@ -20874,8 +20875,8 @@
       </c>
     </row>
     <row r="473" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A473" s="13" t="s">
-        <v>50</v>
+      <c r="A473" t="s">
+        <v>116</v>
       </c>
       <c r="B473" t="s">
         <v>6</v>
@@ -20885,8 +20886,8 @@
       </c>
     </row>
     <row r="474" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A474" s="13" t="s">
-        <v>49</v>
+      <c r="A474" t="s">
+        <v>113</v>
       </c>
       <c r="B474" t="s">
         <v>6</v>
@@ -20896,8 +20897,8 @@
       </c>
     </row>
     <row r="475" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A475" s="13" t="s">
-        <v>48</v>
+      <c r="A475" t="s">
+        <v>110</v>
       </c>
       <c r="B475" t="s">
         <v>6</v>
@@ -20907,8 +20908,8 @@
       </c>
     </row>
     <row r="476" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A476" s="13" t="s">
-        <v>47</v>
+      <c r="A476" t="s">
+        <v>106</v>
       </c>
       <c r="B476" t="s">
         <v>6</v>
@@ -20917,128 +20918,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="477" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A477" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="B477" t="s">
-        <v>6</v>
-      </c>
-      <c r="C477" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="478" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A478" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B478" t="s">
-        <v>6</v>
-      </c>
-      <c r="C478" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="479" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A479" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B479" t="s">
-        <v>6</v>
-      </c>
-      <c r="C479" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="480" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A480" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B480" t="s">
-        <v>6</v>
-      </c>
-      <c r="C480" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="481" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A481" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B481" t="s">
-        <v>6</v>
-      </c>
-      <c r="C481" t="s">
-        <v>1393</v>
-      </c>
-    </row>
-    <row r="482" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A482" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B482" t="s">
-        <v>6</v>
-      </c>
-      <c r="C482" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="483" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A483" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B483" t="s">
-        <v>6</v>
-      </c>
-      <c r="C483" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="484" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A484" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B484" t="s">
-        <v>6</v>
-      </c>
-      <c r="C484" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="485" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A485" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B485" t="s">
-        <v>6</v>
-      </c>
-      <c r="C485" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="486" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A486" s="13" t="s">
-        <v>1395</v>
-      </c>
-      <c r="B486" t="s">
-        <v>6</v>
-      </c>
-      <c r="C486" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="487" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A487" s="13" t="s">
-        <v>1394</v>
-      </c>
-      <c r="B487" t="s">
-        <v>6</v>
-      </c>
-      <c r="C487" t="s">
-        <v>8</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState ref="A2:C476">
+    <sortCondition ref="A2:A476"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>